<commit_message>
Ahora se hizo total y por cuenca, FALTA por tipo de Fluido
</commit_message>
<xml_diff>
--- a/DataBases/BI- Factor Emision  - IPCC - 2006.xlsx
+++ b/DataBases/BI- Factor Emision  - IPCC - 2006.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931E5597-85B0-41DE-8DDE-F8B4B41E821E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323DAAF4-508C-4FF7-B076-FD5ACED6CE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9D32552E-AF3B-45A7-B056-DE9A4E55E1FF}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -449,11 +449,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -489,16 +491,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,6 +516,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1524355</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63A79237-9486-0E09-A0FD-7C81B31E3A5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3590925" y="7591425"/>
+          <a:ext cx="2543530" cy="6506483"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -817,7 +867,7 @@
   <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K13"/>
+      <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3613,8 +3663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111721CC-C809-41EA-9875-1A5F5DBDFCBE}">
   <dimension ref="C4:P44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,13 +3863,16 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
       <c r="G33" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G36" s="8" t="s">
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>128</v>
       </c>
       <c r="H36" s="7">
@@ -3843,8 +3896,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G37" s="8" t="s">
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>77841</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H37" s="7">
@@ -3868,8 +3924,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G38" s="8" t="s">
+    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>0.6</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>129</v>
       </c>
       <c r="H38" s="7">
@@ -3893,7 +3952,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
       <c r="M40" t="s">
         <v>123</v>
       </c>
@@ -3908,7 +3967,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
       <c r="N41" t="s">
         <v>121</v>
       </c>
@@ -3920,7 +3979,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
         <v>122</v>
       </c>
@@ -3935,7 +3994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:16" x14ac:dyDescent="0.25">
       <c r="N44" t="s">
         <v>121</v>
       </c>
@@ -3950,5 +4009,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>